<commit_message>
updated mongodb excel sheet
</commit_message>
<xml_diff>
--- a/docs/features/perf-tuning/Saral App MongoDB Tuning.xlsx
+++ b/docs/features/perf-tuning/Saral App MongoDB Tuning.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Collection Name</t>
   </si>
@@ -27,6 +27,12 @@
   </si>
   <si>
     <t>Shard</t>
+  </si>
+  <si>
+    <t>document examined before no index</t>
+  </si>
+  <si>
+    <t>document examined after</t>
   </si>
   <si>
     <t>Brand</t>
@@ -44,6 +50,44 @@
   </si>
   <si>
     <t>sh.shardCollection("saralv1.5.brands" , { "state" : "hashed", "schoolId":1})</t>
+  </si>
+  <si>
+    <t>state as collspan whereas schoolId
+ doesnot have .when we pass only state
+ then  "docsExamined": 6 are returning
+ when itis passing with schoolId then 
+only 1 doc is returned 
+2. { "state": { $exists: false }} 6 
+documents returned .</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">1. {"state": "up","schoolId": "09670702901"}
+doc examined: 1, index examined: 1
+2. { "state": { $exists: false }} 1 document examined  .
+no call span is present.
+fetch and IXSCAN is found 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>indexing</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve"> on state and schoolId</t>
+    </r>
   </si>
   <si>
     <t>Class</t>
@@ -58,6 +102,40 @@
 4. Mark.deleteMany({ schoolId: req.school.schoolId, studentId: student.studentId }
 5. Student.deleteMany(lookup).lean()
 6. Exam.deleteMany(match)</t>
+  </si>
+  <si>
+    <t>1. {schoolId: u001 } 
+colspan is present ,nReturned =9 
+doc examined = 38</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">1. {schoolId: u001}
+doc examined =9
+doc returned = 9
+no colspan found
+fetch and IXSCAN is present and nreturned is 9 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>indexing</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> on schoolId</t>
+    </r>
   </si>
   <si>
     <t>Counter</t>
@@ -84,6 +162,49 @@
 7. Exam.updateOne(match, update).lean().exec()</t>
   </si>
   <si>
+    <t>1.  {"classId": '2',
+  "schoolId": 'u002',
+  "subject": 'Hindi',
+  "examDate": '11/10/2021'}
+colspan is present
+62 examined
+2. {examId : 12}
+doc examined is 1
+fetch and IXSCAN is present .</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">1.   {
+"classId": '2',
+ "schoolId": 'u002',
+  "subject": 'Hindi',
+  "examDate": '11/10/2021'
+}
+after indexing colspan is not present 
+FETCH AND IXSCAN is present. nReturned :1  1 doc is examined . 1 doc returned
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>indexing</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> on classId, schoolId, subject , examDate</t>
+    </r>
+  </si>
+  <si>
     <t>Lock</t>
   </si>
   <si>
@@ -96,15 +217,8 @@
     <t>marks</t>
   </si>
   <si>
-    <t>1. Mark.findOne({ schoolId: data.schoolId, userId: data.userId, studentId: data.studentId, classId: data.classId, subject: data.subject, examDate: data.examDate, roiId: data.roiId })
-2. Mark.create(data)
-3. Mark.update(lookup, update)
-4. Mark.countDocuments("{}") -? 
-5. Mark.find({}
-6. Exams.find({})
-7. Class.find({})
-8. School.find({})
-9. Mark.find(match)</t>
+    <t>1. {"schoolId": "u001","studentClass":{$elemMatch:{"classId" : "2", "className": "Class-2"}},
+"section": "D"}</t>
   </si>
   <si>
     <t>ROI</t>
@@ -118,6 +232,39 @@
 3. ROI.findOne({ classId: examExist.classId, subject: examExist.subject, state: school.state, type: examExist.type }).lean()
 4. ROI.find(examSetLookupExist, { roiId: 1,roi:1 }).lean()
 5. Counter.findOneAndUpdate(match,update,options)</t>
+  </si>
+  <si>
+    <t>1. {"classId": "2", "subject": "Hindi", "state": "up", "type": "hindi_4s_20q_omr"}
+colspan is present =&gt; nreturned: 1 .
+ doc examined : 69
+doc returned: 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">1. {"classId": "2", "subject": "Hindi", "state": "up", "type": "hindi_4s_20q_omr"}
+colspan is not present . doc examined : 1, doc returned:1
+fetch and IXSCAN is present  and returned 1 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Indexing</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> :- classId,subject,hindi,type</t>
+    </r>
   </si>
   <si>
     <t>School</t>
@@ -153,17 +300,60 @@
 8. Student.updateOne(lookup, updateData).lean().exec()</t>
   </si>
   <si>
+    <t>1. {"schoolId": "u001","studentClass":{$elemMatch:{"classId" : "2", "className": "Class-2"}},
+"section": "D"}
+Collspan is present
+"docsExamined": 346</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">1. {"schoolId": "u001","studentClass":{$elemMatch:{"classId" : "2", "className": "Class-2"}},
+"section": "D"}
+Collspan is not present
+"docReturned" : 5
+"docsExamined": 38
+FETCH : nreturned 5
+IXSCAN: nreturned 5 , multikeyindex :- yes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Indexing</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> :- schoolId , studentClass, section</t>
+    </r>
+  </si>
+  <si>
     <t>User</t>
   </si>
   <si>
     <t>users</t>
+  </si>
+  <si>
+    <t>1.   await Users.findOne({ userId: userId, __v: 0})</t>
+  </si>
+  <si>
+    <t>index {userId: -1 }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -175,8 +365,18 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +387,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF6AA84F"/>
         <bgColor rgb="FF6AA84F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -210,20 +416,26 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -448,7 +660,9 @@
     <col customWidth="1" min="2" max="2" width="17.75"/>
     <col customWidth="1" min="3" max="3" width="132.0"/>
     <col customWidth="1" min="4" max="4" width="28.63"/>
-    <col customWidth="1" min="5" max="5" width="54.88"/>
+    <col customWidth="1" min="5" max="5" width="58.88"/>
+    <col customWidth="1" min="6" max="6" width="68.5"/>
+    <col customWidth="1" min="7" max="7" width="73.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -467,136 +681,180 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="3"/>
+      <c r="F8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
update query in excel
</commit_message>
<xml_diff>
--- a/docs/features/perf-tuning/Saral App MongoDB Tuning.xlsx
+++ b/docs/features/perf-tuning/Saral App MongoDB Tuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\react-native\Project-Saral\docs\features\perf-tuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34944581-B563-4D74-B84B-4EC3A1B3EF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620E3792-3C44-4264-B62B-C8A75D663B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,10 +128,6 @@
     <t>marks</t>
   </si>
   <si>
-    <t>1. {"schoolId": "u001","studentClass":{$elemMatch:{"classId" : "2", "className": "Class-2"}},
-"section": "D"}</t>
-  </si>
-  <si>
     <t>ROI</t>
   </si>
   <si>
@@ -271,6 +267,9 @@
   </si>
   <si>
     <t>userld is unique key so doc examined was 1 and returned also 1</t>
+  </si>
+  <si>
+    <t>1 Marks.bulkWrite(updates)     2.  Marks.find(match)</t>
   </si>
 </sst>
 </file>
@@ -402,7 +401,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -626,13 +625,15 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="132" customWidth="1"/>
+    <col min="3" max="3" width="98" customWidth="1"/>
     <col min="4" max="4" width="30.77734375" customWidth="1"/>
     <col min="5" max="5" width="58.88671875" customWidth="1"/>
     <col min="6" max="6" width="56.88671875" customWidth="1"/>
@@ -670,10 +671,10 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
@@ -682,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="92.4" x14ac:dyDescent="0.25">
@@ -696,17 +697,17 @@
         <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -730,17 +731,17 @@
         <v>20</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -752,7 +753,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -760,7 +761,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -768,86 +769,86 @@
     </row>
     <row r="8" spans="1:7" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="D8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="118.8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="C9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="132" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="D11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update index folderfor excel
</commit_message>
<xml_diff>
--- a/docs/features/perf-tuning/Saral App MongoDB Tuning.xlsx
+++ b/docs/features/perf-tuning/Saral App MongoDB Tuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\react-native\Project-Saral\docs\features\perf-tuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620E3792-3C44-4264-B62B-C8A75D663B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F913E094-9315-4192-856B-80C662CCA910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t>Collection Name</t>
   </si>
@@ -196,12 +196,6 @@
 </t>
   </si>
   <si>
-    <t>state and schoolId</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> schoolId</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. {schoolId: u001}
 doc examined =9
 doc returned = 9
@@ -221,9 +215,6 @@
 </t>
   </si>
   <si>
-    <t>classId, schoolId, subject , examDate</t>
-  </si>
-  <si>
     <t>1. School.findOne({ schoolId: users.schoolId }
 2. classes.find({ schoolId }
 3. School.findOne({ schoolId: req.params.schoolId.toLowerCase() }
@@ -235,9 +226,6 @@
 9. School.updateOne(lookup, update).lean().exec()"</t>
   </si>
   <si>
-    <t>schoolId</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. {"schoolId": "u001","studentClass":{$elemMatch:{"classId" : "2", "className": "Class-2"}},
 "section": "D"}
 Collspan is not present
@@ -248,21 +236,12 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> schoolId , studentClass, section</t>
-  </si>
-  <si>
-    <t>userId</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. {"classId": "2", "subject": "Hindi", "state": "up", "type": "hindi_4s_20q_omr"}
 colspan is not present . doc examined : 1, doc returned:1
 fetch and IXSCAN is present  and returned 1 
 </t>
   </si>
   <si>
-    <t>classId,subject,hindi,type</t>
-  </si>
-  <si>
     <t>schoold is unique key so doc examined was 1 and returned also 1</t>
   </si>
   <si>
@@ -270,6 +249,26 @@
   </si>
   <si>
     <t>1 Marks.bulkWrite(updates)     2.  Marks.find(match)</t>
+  </si>
+  <si>
+    <t>{schoolId: -1}</t>
+  </si>
+  <si>
+    <t>{schoolId: -1, "studentClass.classId": -1,
+    "studentClass.className": -1,section: -1}</t>
+  </si>
+  <si>
+    <t>{classId: -1, subject: -1, state: -1, type: -1}</t>
+  </si>
+  <si>
+    <t>{userId: -1}</t>
+  </si>
+  <si>
+    <t>{state:-1, schoolId: -1}</t>
+  </si>
+  <si>
+    <t>{classId: -1, schoolId: -1, subject: -1, examDate: -1,examId: -1
+}</t>
   </si>
 </sst>
 </file>
@@ -625,8 +624,8 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -634,7 +633,7 @@
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="98" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
     <col min="5" max="5" width="58.88671875" customWidth="1"/>
     <col min="6" max="6" width="56.88671875" customWidth="1"/>
     <col min="7" max="7" width="55.109375" customWidth="1"/>
@@ -674,7 +673,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
@@ -697,14 +696,14 @@
         <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -730,15 +729,15 @@
       <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>45</v>
+      <c r="D5" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -761,7 +760,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -778,14 +777,14 @@
         <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="4" t="s">
         <v>29</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="118.8" x14ac:dyDescent="0.25">
@@ -796,17 +795,17 @@
         <v>31</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="132" x14ac:dyDescent="0.25">
@@ -819,15 +818,15 @@
       <c r="C10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>49</v>
+      <c r="D10" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
@@ -841,14 +840,14 @@
         <v>38</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>